<commit_message>
dialog done for lesson 2
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/Speaking_dialogs.xlsx
+++ b/public/docs/Excel data/Speaking_dialogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D455273A-8DFA-4F5C-800A-2F1DD49B1ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9DF162-40EC-482E-B71B-AC4591E3E32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="12264" activeTab="1" xr2:uid="{C0062FF2-E2FC-4C90-8934-4D3B04DA67C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0062FF2-E2FC-4C90-8934-4D3B04DA67C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="74">
   <si>
     <t>[</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>Так, мені вона дуже подобається.</t>
+  </si>
+  <si>
+    <t>What time do you wake up?</t>
+  </si>
+  <si>
+    <t>I wake up at 7 a.m.</t>
+  </si>
+  <si>
+    <t>О котрій ти прокидаєшся?</t>
+  </si>
+  <si>
+    <t>Я прокидаюся о 7-й ранку.</t>
   </si>
 </sst>
 </file>
@@ -643,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FBB4F4-1DC4-405A-8B2E-13838DF638AC}">
   <dimension ref="B2:K360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,21 +985,33 @@
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
       <c r="D16" t="s">
         <v>35</v>
       </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
       <c r="F16" t="s">
         <v>3</v>
       </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
       <c r="H16" t="s">
         <v>36</v>
       </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
       <c r="J16" t="s">
         <v>4</v>
       </c>
       <c r="K16" t="str">
-        <f>B16&amp;C16&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16&amp;J16</f>
-        <v>{question: "", q_translate: "", answer: "", a_translate: ""},</v>
+        <f>B16&amp;C16&amp;I15&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16&amp;J16</f>
+        <v>{question: "О котрій ти прокидаєшся?", q_translate: "What time do you wake up?", answer: "Я прокидаюся о 7-й ранку.", a_translate: "I wake up at 7 a.m."},</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
@@ -1007,8 +1031,8 @@
         <v>4</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:K23" si="2">B17&amp;C17&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17&amp;J17</f>
-        <v>{question: "", q_translate: "", answer: "", a_translate: ""},</v>
+        <f>B17&amp;I16&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17&amp;J17</f>
+        <v>{question: "I wake up at 7 a.m.", q_translate: "", answer: "", a_translate: ""},</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
@@ -1028,7 +1052,7 @@
         <v>4</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K17:K23" si="2">B18&amp;C18&amp;D18&amp;E18&amp;F18&amp;G18&amp;H18&amp;I18&amp;J18</f>
         <v>{question: "", q_translate: "", answer: "", a_translate: ""},</v>
       </c>
     </row>
@@ -6617,7 +6641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBC2EAC-9E30-4B81-8AEA-684BA5F6B338}">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>